<commit_message>
[Github Action: dev]: Adding excel lineage report
</commit_message>
<xml_diff>
--- a/output_dev/lineage_customer_orders_demo.xlsx
+++ b/output_dev/lineage_customer_orders_demo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1247,91 +1247,10 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>first_name</t>
+          <t>orders</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>spark_catalog</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>prophecy_demos</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>report_table</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr">
-        <is>
-          <t>full_name</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="inlineStr">
-        <is>
-          <t>full_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>spark_catalog</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>prophecy_demos</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>report_table</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="inlineStr">
-        <is>
-          <t>last_name</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="inlineStr">
-        <is>
-          <t>last_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>spark_catalog</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>prophecy_demos</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>report_table</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr">
-        <is>
-          <t>orders</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="inlineStr">
         <is>
           <t>orders</t>
         </is>

</xml_diff>